<commit_message>
removed non-existent class from pre-req file
</commit_message>
<xml_diff>
--- a/data/rank-prerequisites.xlsx
+++ b/data/rank-prerequisites.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{BADBECB3-5580-4A1B-AEF0-CD93FC166C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACF952DC-D089-4037-9503-220922C331BA}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heyyo\Documents\GitHub\TestMerge\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0E2164-9DC5-4ABA-8D5A-CBFDFFA5FA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Rank</t>
   </si>
@@ -62,16 +67,13 @@
   </si>
   <si>
     <t>ECE*3221</t>
-  </si>
-  <si>
-    <t>SWE*1103</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -461,7 +463,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -475,7 +477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -484,11 +486,6 @@
       </c>
       <c r="D4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>